<commit_message>
Spårspärr and Skarv update
</commit_message>
<xml_diff>
--- a/DataMappingExperiments/Testdata/Fln-Blg Spårspärrar Detaljlägen.xlsx
+++ b/DataMappingExperiments/Testdata/Fln-Blg Spårspärrar Detaljlägen.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\DOK\Anda Nät Anl NJDB NTL\Migrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fresan\Documents\Visual Studio 2015\Projects\DataMappingExperiments\DataMappingExperiments\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20955" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20952" windowHeight="12372"/>
   </bookViews>
   <sheets>
     <sheet name="Resultat" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="158">
   <si>
     <t>Objtypnr</t>
   </si>
@@ -502,12 +502,15 @@
   </si>
   <si>
     <t>2017-02-09 13:20</t>
+  </si>
+  <si>
+    <t>Modell Definition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -835,67 +838,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>48</v>
       </c>
       <c r="AX1" s="5" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="AY1" s="5" t="s">
         <v>49</v>
@@ -1053,7 +1056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10015</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10015</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10015</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10015</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10015</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10015</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10015</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10015</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10015</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10015</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10015</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10015</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10015</v>
       </c>
@@ -3068,7 +3071,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10015</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10015</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10015</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10015</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10015</v>
       </c>
@@ -3843,7 +3846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10015</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10015</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10015</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10015</v>
       </c>
@@ -4463,7 +4466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10015</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10015</v>
       </c>
@@ -4773,7 +4776,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10015</v>
       </c>
@@ -4928,7 +4931,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10015</v>
       </c>
@@ -5083,7 +5086,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10015</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10015</v>
       </c>
@@ -5393,7 +5396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10015</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10015</v>
       </c>
@@ -5703,7 +5706,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10015</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10015</v>
       </c>
@@ -6013,7 +6016,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10015</v>
       </c>
@@ -6168,7 +6171,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10015</v>
       </c>
@@ -6323,7 +6326,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10015</v>
       </c>
@@ -6478,7 +6481,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10015</v>
       </c>
@@ -6633,7 +6636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10015</v>
       </c>
@@ -6788,7 +6791,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10015</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10015</v>
       </c>
@@ -7098,7 +7101,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10015</v>
       </c>
@@ -7253,7 +7256,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10015</v>
       </c>
@@ -7408,7 +7411,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10015</v>
       </c>
@@ -7563,7 +7566,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10015</v>
       </c>
@@ -7718,7 +7721,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10015</v>
       </c>
@@ -7873,7 +7876,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10015</v>
       </c>
@@ -8028,7 +8031,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10015</v>
       </c>
@@ -8183,7 +8186,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10015</v>
       </c>
@@ -8338,7 +8341,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10015</v>
       </c>
@@ -8493,7 +8496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10015</v>
       </c>
@@ -8648,7 +8651,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10015</v>
       </c>
@@ -8803,7 +8806,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10015</v>
       </c>
@@ -8958,7 +8961,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10015</v>
       </c>
@@ -9113,7 +9116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>10015</v>
       </c>
@@ -9268,7 +9271,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10015</v>
       </c>
@@ -9423,7 +9426,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10015</v>
       </c>
@@ -9578,7 +9581,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10015</v>
       </c>
@@ -9733,7 +9736,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10015</v>
       </c>
@@ -9888,7 +9891,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10015</v>
       </c>
@@ -10043,7 +10046,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10015</v>
       </c>
@@ -10198,7 +10201,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>10015</v>
       </c>
@@ -10353,7 +10356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>10015</v>
       </c>
@@ -10508,7 +10511,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10015</v>
       </c>
@@ -10663,7 +10666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>10015</v>
       </c>
@@ -10818,7 +10821,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>10015</v>
       </c>
@@ -10973,7 +10976,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>10015</v>
       </c>
@@ -11128,7 +11131,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>10015</v>
       </c>
@@ -11283,7 +11286,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>10015</v>
       </c>
@@ -11438,7 +11441,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10015</v>
       </c>
@@ -11593,7 +11596,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10015</v>
       </c>
@@ -11748,7 +11751,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10015</v>
       </c>
@@ -11903,7 +11906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10015</v>
       </c>
@@ -12058,7 +12061,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10015</v>
       </c>
@@ -12213,7 +12216,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10015</v>
       </c>
@@ -12368,7 +12371,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10015</v>
       </c>
@@ -12523,7 +12526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10015</v>
       </c>
@@ -12678,7 +12681,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10015</v>
       </c>
@@ -12833,7 +12836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10015</v>
       </c>
@@ -12988,7 +12991,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>10015</v>
       </c>
@@ -13143,7 +13146,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10015</v>
       </c>
@@ -13298,7 +13301,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>10015</v>
       </c>
@@ -13453,7 +13456,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>10015</v>
       </c>
@@ -13608,7 +13611,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10015</v>
       </c>
@@ -13763,7 +13766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>10015</v>
       </c>
@@ -13918,7 +13921,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>10015</v>
       </c>
@@ -14089,14 +14092,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>147</v>
       </c>
@@ -14116,7 +14119,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>65</v>
       </c>
@@ -14136,7 +14139,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>148</v>
       </c>
@@ -14156,7 +14159,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>149</v>
       </c>
@@ -14176,7 +14179,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>149</v>
       </c>
@@ -14196,7 +14199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>149</v>
       </c>
@@ -14216,7 +14219,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>149</v>
       </c>
@@ -14236,7 +14239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>149</v>
       </c>
@@ -14256,7 +14259,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>149</v>
       </c>
@@ -14276,7 +14279,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>149</v>
       </c>
@@ -14296,7 +14299,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>149</v>
       </c>
@@ -14316,7 +14319,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>149</v>
       </c>
@@ -14336,7 +14339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>149</v>
       </c>
@@ -14356,7 +14359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>149</v>
       </c>
@@ -14376,7 +14379,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>149</v>
       </c>
@@ -14396,7 +14399,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>149</v>
       </c>
@@ -14416,7 +14419,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>149</v>
       </c>
@@ -14436,7 +14439,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>149</v>
       </c>
@@ -14456,7 +14459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>149</v>
       </c>
@@ -14476,7 +14479,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>149</v>
       </c>
@@ -14496,7 +14499,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>149</v>
       </c>
@@ -14516,7 +14519,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>149</v>
       </c>
@@ -14536,7 +14539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>149</v>
       </c>
@@ -14556,7 +14559,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>149</v>
       </c>
@@ -14576,7 +14579,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>149</v>
       </c>
@@ -14596,7 +14599,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>149</v>
       </c>
@@ -14616,7 +14619,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>65</v>
       </c>
@@ -14636,7 +14639,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>150</v>
       </c>
@@ -14656,7 +14659,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>52</v>
       </c>
@@ -14676,7 +14679,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>89</v>
       </c>
@@ -14696,7 +14699,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -14719,7 +14722,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14731,7 +14734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14743,7 +14746,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>